<commit_message>
final mods and documentation for behavior modality
</commit_message>
<xml_diff>
--- a/templates/input_behavior.xlsx
+++ b/templates/input_behavior.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\nwb\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Songmao\CURBIO_SL_DK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622DEC72-BFAB-41CF-B8FC-6764CF7B6730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A1D574-9CB5-459A-B8A7-B14EAFA156FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32385" yWindow="1860" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="auto" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>session_id</t>
   </si>
@@ -81,12 +92,6 @@
     <t>SLR087</t>
   </si>
   <si>
-    <t>sensor_mode</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>ch3_in_36data</t>
   </si>
   <si>
@@ -105,9 +110,6 @@
     <t>HeadSensor|TorsoSensor|Breathing</t>
   </si>
   <si>
-    <t>CURBIO_SL_DK/Data/SLR087</t>
-  </si>
-  <si>
     <t>LabChart-BNO055-Basler</t>
   </si>
   <si>
@@ -120,12 +122,6 @@
     <t>LCmat_sampling_rate</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>supplemental_annotation</t>
-  </si>
-  <si>
     <t>Rat forages in open arena</t>
   </si>
   <si>
@@ -144,16 +140,40 @@
     <t>P252D</t>
   </si>
   <si>
+    <t>experimenters</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
     <t>Liao, Song-Mao</t>
   </si>
   <si>
-    <t>experimenters</t>
-  </si>
-  <si>
-    <t>institution</t>
-  </si>
-  <si>
     <t>UC San Diego</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>video_sampling_rate</t>
+  </si>
+  <si>
+    <t>processing_file</t>
+  </si>
+  <si>
+    <t>analysis_file</t>
+  </si>
+  <si>
+    <t>notes_file</t>
+  </si>
+  <si>
+    <t>sensor_description</t>
+  </si>
+  <si>
+    <t>stimulus_notes_file</t>
+  </si>
+  <si>
+    <t>Torso angles (Y, P, R) = (1, 2, 3) columns | Head angles (Y, P, R) = first 3 columns of the second half columns</t>
   </si>
 </sst>
 </file>
@@ -178,7 +198,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +209,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -204,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -212,7 +238,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -597,202 +626,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="26" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29" style="2" customWidth="1"/>
-    <col min="25" max="25" width="49.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="1016" width="8.7109375" style="2"/>
-    <col min="1017" max="1019" width="11.5703125" style="2" customWidth="1"/>
-    <col min="1020" max="16384" width="8.7109375" style="2"/>
+    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="90.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="57.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="43.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="1015" width="8.7109375" style="2"/>
+    <col min="1016" max="1018" width="11.5703125" style="2" customWidth="1"/>
+    <col min="1019" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="3">
+        <v>268</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4">
+        <v>43028</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="str">
+        <f>"/net/birdstore/Songmao/CURBIO_SL_DK/Data/"&amp;B2</f>
+        <v>/net/birdstore/Songmao/CURBIO_SL_DK/Data/SLR087</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="P2" s="4">
+        <v>43287</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>40000</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="3">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="3">
-        <v>43287</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="2">
-        <v>268</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="3">
-        <v>43028</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2" s="2">
-        <v>40000</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>31</v>
+      <c r="AB2" s="3" t="str">
+        <f>B2&amp;"_D_pcts.csv"</f>
+        <v>SLR087_D_pcts.csv</v>
+      </c>
+      <c r="AC2" s="3" t="str">
+        <f>A2&amp;"_D_bBoolsMat.mat"</f>
+        <v>SLR087_arena_d1_D_bBoolsMat.mat</v>
+      </c>
+      <c r="AD2" s="3" t="str">
+        <f>A2&amp;"_D_NWBFile_notes.csv"</f>
+        <v>SLR087_arena_d1_D_NWBFile_notes.csv</v>
+      </c>
+      <c r="AE2" s="3" t="str">
+        <f>A2&amp;"_D_NWBFile_stimulus_notes.csv"</f>
+        <v>SLR087_arena_d1_D_NWBFile_stimulus_notes.csv</v>
       </c>
     </row>
   </sheetData>

</xml_diff>